<commit_message>
one excel file is modified and added
</commit_message>
<xml_diff>
--- a/Hometown Scenario.xlsx
+++ b/Hometown Scenario.xlsx
@@ -1,66 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CBT\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Functional" sheetId="1" r:id="rId1"/>
     <sheet name="Integration" sheetId="3" r:id="rId2"/>
     <sheet name="End to end " sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>CBT</author>
-  </authors>
-  <commentList>
-    <comment ref="M1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CBT:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="266">
   <si>
     <t>Sl no</t>
   </si>
@@ -1150,12 +1113,18 @@
   <si>
     <t>Home Décor item is sorted based on Discount</t>
   </si>
+  <si>
+    <t>home item select</t>
+  </si>
+  <si>
+    <t>shipping address</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1185,19 +1154,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1544,21 +1500,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
@@ -1569,7 +1525,7 @@
     <col min="7" max="13" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1607,7 +1563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="90">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1643,7 +1599,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="105">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1679,7 +1635,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="105">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1715,7 +1671,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="75">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1751,7 +1707,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="90">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1787,7 +1743,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="90">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1823,7 +1779,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="90">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1859,7 +1815,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="75">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1895,7 +1851,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1931,7 +1887,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="75">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1967,7 +1923,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="90">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2003,7 +1959,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="90">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2039,7 +1995,7 @@
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="75">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2075,7 +2031,7 @@
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="75">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2111,7 +2067,7 @@
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="75">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2147,7 +2103,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="75">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2183,7 +2139,7 @@
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="75">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2219,7 +2175,7 @@
       </c>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="75">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2255,7 +2211,7 @@
       </c>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="90">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2291,7 +2247,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="75">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2334,14 +2290,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
@@ -2352,7 +2308,7 @@
     <col min="13" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2399,7 +2355,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="165">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2431,7 +2387,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="135">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2463,7 +2419,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="150">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2495,7 +2451,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="180">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2527,7 +2483,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="180">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2559,7 +2515,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="120">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2591,7 +2547,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="105">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2623,7 +2579,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="135">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2655,7 +2611,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="135">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2687,7 +2643,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="135">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2719,7 +2675,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2733,7 +2689,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2747,7 +2703,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2761,7 +2717,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2775,7 +2731,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2789,7 +2745,7 @@
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2803,7 +2759,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2817,7 +2773,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -2831,7 +2787,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2845,7 +2801,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2859,7 +2815,7 @@
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2873,7 +2829,7 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2887,7 +2843,7 @@
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2901,7 +2857,7 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2915,7 +2871,7 @@
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2929,7 +2885,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2943,7 +2899,7 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2957,7 +2913,7 @@
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2974,19 +2930,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
@@ -3002,7 +2957,7 @@
     <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3049,7 +3004,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="330">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3081,7 +3036,7 @@
       </c>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="285" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="285">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3113,7 +3068,7 @@
       </c>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="345" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="345">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3145,7 +3100,7 @@
       </c>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="345" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="345">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3177,7 +3132,7 @@
       </c>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="300" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="300">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3209,7 +3164,7 @@
       </c>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="409.5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3241,7 +3196,7 @@
       </c>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="409.5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3273,7 +3228,7 @@
       </c>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="330" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="330">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3305,7 +3260,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="409.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3337,7 +3292,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:15" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="409.5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3369,7 +3324,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="1:15" ht="240" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="240">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3401,7 +3356,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="1:15" ht="360" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="360">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3433,7 +3388,7 @@
       </c>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="1:15" ht="315" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="315">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3465,7 +3420,7 @@
       </c>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:15" ht="390" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="390">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3497,7 +3452,7 @@
       </c>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:15" ht="405" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="405">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3529,7 +3484,7 @@
       </c>
       <c r="L16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="360" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="360">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3561,7 +3516,7 @@
       </c>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="405" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="405">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3593,7 +3548,7 @@
       </c>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="345" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="345">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3625,7 +3580,7 @@
       </c>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="409.5" customHeight="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3657,7 +3612,7 @@
       </c>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="409.5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3689,7 +3644,7 @@
       </c>
       <c r="L21" s="4"/>
     </row>
-    <row r="22" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="409.5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3719,7 +3674,7 @@
       </c>
       <c r="L22" s="4"/>
     </row>
-    <row r="23" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="409.5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3751,7 +3706,7 @@
       </c>
       <c r="L23" s="4"/>
     </row>
-    <row r="24" spans="1:12" ht="360" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="360">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3783,7 +3738,7 @@
       </c>
       <c r="L24" s="4"/>
     </row>
-    <row r="25" spans="1:12" ht="405" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="405">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3811,7 +3766,7 @@
       </c>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" ht="301.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="301.5" customHeight="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3839,7 +3794,7 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="44.25" customHeight="1">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3869,23 +3824,35 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="409.5">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="B28" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3899,7 +3866,7 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3913,7 +3880,7 @@
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3927,7 +3894,7 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3941,7 +3908,7 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3955,7 +3922,7 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3969,7 +3936,7 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3987,4 +3954,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>